<commit_message>
add import csv, category
</commit_message>
<xml_diff>
--- a/products1.xlsx
+++ b/products1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenServer\domains\scrapping-brain\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OSPanel\domains\scrapping-brain\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Аркуш1!$A$1:$AD$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Аркуш1!$A$1:$AD$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
   <si>
     <t>CategoryID</t>
   </si>
@@ -125,160 +125,148 @@
     <t>FOP</t>
   </si>
   <si>
-    <t>4444</t>
-  </si>
-  <si>
-    <t>Пристрої безперебійного живлення</t>
-  </si>
-  <si>
-    <t>SC620I</t>
-  </si>
-  <si>
-    <t>APC</t>
-  </si>
-  <si>
-    <t>Smart-UPS SC 620VA</t>
-  </si>
-  <si>
-    <t>Пристрій безперебійного живлення Smart-UPS SC 620VA APC (SC620I)</t>
-  </si>
-  <si>
-    <t>для відеоспостереження, для домашніх ПК, з автоматичною стабілізацією, лінійно-інтерактивний (line interactive), 400 Вт, 620 В*А, апроксимована синусоїда, 151 до 320 В, RBC4, 119х168х368, 12.3 кг</t>
-  </si>
-  <si>
-    <t>Пристрої бесперебійного живлення</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>https://opt.brain.com.ua/Pristriy_bezperebiynogo_jhivlennya_APC_Smart-UPS_SC_620VA_SC620I-p23160.html</t>
-  </si>
-  <si>
-    <t>8504403000</t>
-  </si>
-  <si>
-    <t>Пристрій безперебійного живлення</t>
-  </si>
-  <si>
-    <t>Тайвань</t>
-  </si>
-  <si>
-    <t>ET01833</t>
-  </si>
-  <si>
-    <t>Флеш-накопичувачі</t>
-  </si>
-  <si>
-    <t>TS32GCF133</t>
-  </si>
-  <si>
-    <t>Transcend</t>
-  </si>
-  <si>
-    <t>32Gb Compact Flash  133x</t>
-  </si>
-  <si>
-    <t>Карта пам'яті Transcend 32Gb Compact Flash 133x (TS32GCF133)</t>
-  </si>
-  <si>
-    <t>Compact Flash, 32 ГБ</t>
-  </si>
-  <si>
-    <t>Карти пам'яті</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
-    <t>https://opt.brain.com.ua/Flesh_karta_Transcend_32Gb_Compact_Flash_133x_TS32GCF133-p22484.html</t>
-  </si>
-  <si>
-    <t>8523511000</t>
-  </si>
-  <si>
-    <t>Карта пам'яті</t>
-  </si>
-  <si>
     <t>Китай</t>
   </si>
   <si>
-    <t>ET00808</t>
-  </si>
-  <si>
-    <t>TS16GCF133</t>
-  </si>
-  <si>
-    <t>16Gb Compact Flash 133x</t>
-  </si>
-  <si>
-    <t>Карта пам'яті Transcend 16Gb Compact Flash 133x (TS16GCF133)</t>
-  </si>
-  <si>
-    <t>Compact Flash, 16 ГБ</t>
-  </si>
-  <si>
-    <t>https://opt.brain.com.ua/Flesh_karta_Transcend_16Gb_Compact_Flash_133x_TS16GCF133-p22483.html</t>
-  </si>
-  <si>
-    <t>ET00365</t>
-  </si>
-  <si>
-    <t>TS8GCF133</t>
-  </si>
-  <si>
-    <t>8Gb Compact Flash 133x</t>
-  </si>
-  <si>
-    <t>Карта пам'яті Transcend 8Gb Compact Flash 133x (TS8GCF133)</t>
-  </si>
-  <si>
-    <t>Compact Flash, 8 ГБ</t>
-  </si>
-  <si>
-    <t>https://opt.brain.com.ua/Flesh_karta_Transcend_8Gb_Compact_Flash_133x_TS8GCF133-p20732.html</t>
-  </si>
-  <si>
-    <t>KM09044</t>
-  </si>
-  <si>
-    <t>Акустичні системи</t>
-  </si>
-  <si>
-    <t>980-000029</t>
-  </si>
-  <si>
     <t>Logitech</t>
   </si>
   <si>
-    <t>S-150 Black</t>
-  </si>
-  <si>
-    <t>Акустична система Logitech S-150 Black (980-000029)</t>
-  </si>
-  <si>
-    <t>дротове, 2.0, USB, Потужність, Вт - 1.2, пластик, комп'ютерні колонки</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>https://opt.brain.com.ua/Akustichna_sistema_Logitech_S-150_Black_980-000029-p25940.html</t>
-  </si>
-  <si>
-    <t>8518210090</t>
-  </si>
-  <si>
-    <t>Акустична система</t>
+    <t>B0005197</t>
+  </si>
+  <si>
+    <t>Маніпулятори</t>
+  </si>
+  <si>
+    <t>920-002643</t>
+  </si>
+  <si>
+    <t>K120 Ukr</t>
+  </si>
+  <si>
+    <t>Клавіатура Logitech K120 Ukr (920-002643)</t>
+  </si>
+  <si>
+    <t>конструкція - мембранна, USB, англійська, українська, повнорозмірна, Клавіш - 104, вологостійкість, безшумне введення, Колір - чорний</t>
+  </si>
+  <si>
+    <t>Клавіатури</t>
+  </si>
+  <si>
+    <t>https://opt.brain.com.ua/Klaviatura_Logitech_K120_920-002643-p47223.html</t>
+  </si>
+  <si>
+    <t>8471606000</t>
+  </si>
+  <si>
+    <t>Клавіатура</t>
+  </si>
+  <si>
+    <t>418</t>
+  </si>
+  <si>
+    <t>Витратні матеріали оригінальні</t>
+  </si>
+  <si>
+    <t>51645AE</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>DJ No. 45 Black</t>
+  </si>
+  <si>
+    <t>Картридж HP DJ No. 45 Black (51645AE)</t>
+  </si>
+  <si>
+    <t>струменевий, оригінальний, Black, Сумісність - Hewlett Packard</t>
+  </si>
+  <si>
+    <t>Картриджі</t>
+  </si>
+  <si>
+    <t>https://opt.brain.com.ua/Kartridjh_HP_DJ_No_45_Black_51645AE-p19822.html</t>
+  </si>
+  <si>
+    <t>8443999090</t>
+  </si>
+  <si>
+    <t>Картридж</t>
+  </si>
+  <si>
+    <t>S0007198</t>
+  </si>
+  <si>
+    <t>CH561HE</t>
+  </si>
+  <si>
+    <t>DJ No.122 Black, DJ 2050</t>
+  </si>
+  <si>
+    <t>Картридж HP DJ No.122 Black, DJ 2050 (CH561HE)</t>
+  </si>
+  <si>
+    <t>струменевий, оригінальний, Black, Сумісність - Hewlett Packard, 120 стр</t>
+  </si>
+  <si>
+    <t>https://opt.brain.com.ua/Kartridjh_HP_DJ_No122_Black_DJ_2050_CH561HE-p36184.html</t>
+  </si>
+  <si>
+    <t>S0007216</t>
+  </si>
+  <si>
+    <t>CH562HE</t>
+  </si>
+  <si>
+    <t>DJ No.122 color, DJ 2050</t>
+  </si>
+  <si>
+    <t>Картридж HP DJ No.122 color, DJ 2050 (CH562HE)</t>
+  </si>
+  <si>
+    <t>струменевий, оригінальний, Color, Сумісність - Hewlett Packard, 100 стр</t>
+  </si>
+  <si>
+    <t>https://opt.brain.com.ua/Kartridjh_HP_DJ_No122_color_DJ_2050_CH562HE-p36226.html</t>
+  </si>
+  <si>
+    <t>3215902000</t>
+  </si>
+  <si>
+    <t>KM09159</t>
+  </si>
+  <si>
+    <t>2146B001/2146B005/21460001</t>
+  </si>
+  <si>
+    <t>Canon</t>
+  </si>
+  <si>
+    <t>CL-38 Color</t>
+  </si>
+  <si>
+    <t>Картридж CL-38 Color Canon (2146B001/2146B005/21460001)</t>
+  </si>
+  <si>
+    <t>струменевий, оригінальний, Magenta, Yellow, Cyan, Сумісність - Canon, 205 стр</t>
+  </si>
+  <si>
+    <t>https://opt.brain.com.ua/Kartridjh_CANON_CL-38_Color_2146B001_2146B005_21460001-p19728.html</t>
   </si>
 </sst>
 </file>
@@ -635,7 +623,7 @@
   <dimension ref="A1:AD6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,125 +725,125 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>7273</v>
+        <v>1269</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="I2">
-        <v>376</v>
+        <v>8.6</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>369</v>
       </c>
       <c r="N2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="O2" s="1">
         <v>24</v>
       </c>
       <c r="P2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="Q2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="R2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="S2" s="1">
-        <v>17</v>
+        <v>158</v>
       </c>
       <c r="T2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="U2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="V2" s="1">
-        <v>1035</v>
+        <v>1011</v>
       </c>
       <c r="W2" s="1">
-        <v>166</v>
+        <v>67</v>
       </c>
       <c r="X2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="Y2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="Z2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="AA2">
-        <v>14060</v>
+        <v>369</v>
       </c>
       <c r="AB2">
         <v>0</v>
       </c>
       <c r="AC2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="AD2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1260</v>
+        <v>7925</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I3">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -864,72 +852,70 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="1">
-        <v>60</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="O3" s="1"/>
       <c r="P3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="Q3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="R3" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="S3" s="1">
-        <v>27</v>
+        <v>218</v>
       </c>
       <c r="T3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="U3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="V3" s="1">
-        <v>1060</v>
+        <v>1034</v>
       </c>
       <c r="W3" s="1">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="X3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Y3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="Z3" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="AA3">
-        <v>999</v>
+        <v>2844</v>
       </c>
       <c r="AB3">
         <v>0</v>
       </c>
       <c r="AC3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="AD3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1260</v>
+        <v>7925</v>
       </c>
       <c r="B4" t="s">
         <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
         <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
         <v>60</v>
@@ -941,11 +927,11 @@
         <v>62</v>
       </c>
       <c r="I4">
-        <v>21</v>
+        <v>18.39</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -954,72 +940,70 @@
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O4" s="1">
-        <v>60</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="O4" s="1"/>
       <c r="P4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="Q4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="R4" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="S4" s="1">
-        <v>29</v>
+        <v>239</v>
       </c>
       <c r="T4" t="s">
         <v>63</v>
       </c>
       <c r="U4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="V4" s="1">
-        <v>1060</v>
+        <v>1034</v>
       </c>
       <c r="W4" s="1">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="X4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Y4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="Z4" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="AA4">
-        <v>856</v>
+        <v>691</v>
       </c>
       <c r="AB4">
         <v>0</v>
       </c>
       <c r="AC4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="AD4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>1260</v>
+        <v>7925</v>
       </c>
       <c r="B5" t="s">
         <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
         <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
         <v>66</v>
@@ -1031,11 +1015,11 @@
         <v>68</v>
       </c>
       <c r="I5">
-        <v>18</v>
+        <v>20.2</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -1044,66 +1028,64 @@
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>38</v>
-      </c>
-      <c r="O5" s="1">
-        <v>60</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="O5" s="1"/>
       <c r="P5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="Q5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="R5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="S5" s="1">
-        <v>30</v>
+        <v>240</v>
       </c>
       <c r="T5" t="s">
         <v>69</v>
       </c>
       <c r="U5" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="V5" s="1">
-        <v>1060</v>
+        <v>1034</v>
       </c>
       <c r="W5" s="1">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="X5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Y5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="Z5" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="AA5">
-        <v>709</v>
+        <v>798</v>
       </c>
       <c r="AB5">
         <v>0</v>
       </c>
       <c r="AC5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="AD5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>1038</v>
+        <v>7925</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
         <v>72</v>
@@ -1121,72 +1103,70 @@
         <v>76</v>
       </c>
       <c r="I6">
-        <v>21</v>
+        <v>20.75</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>899</v>
+        <v>0</v>
       </c>
       <c r="N6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="1"/>
+      <c r="P6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R6" t="s">
+        <v>30</v>
+      </c>
+      <c r="S6" s="1">
+        <v>320</v>
+      </c>
+      <c r="T6" t="s">
         <v>77</v>
       </c>
-      <c r="O6" s="1">
-        <v>12</v>
-      </c>
-      <c r="P6" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>39</v>
-      </c>
-      <c r="R6" t="s">
-        <v>78</v>
-      </c>
-      <c r="S6" s="1">
-        <v>80</v>
-      </c>
-      <c r="T6" t="s">
-        <v>79</v>
-      </c>
       <c r="U6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="V6" s="1">
-        <v>1012</v>
+        <v>1034</v>
       </c>
       <c r="W6" s="1">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="X6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="Y6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Z6" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="AA6">
-        <v>899</v>
+        <v>795</v>
       </c>
       <c r="AB6">
         <v>0</v>
       </c>
       <c r="AC6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="AD6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AD6"/>
+  <autoFilter ref="A1:AD1"/>
   <sortState ref="A2:AD63585">
     <sortCondition descending="1" ref="A1"/>
   </sortState>

</xml_diff>